<commit_message>
grafico dos algoritmos python
</commit_message>
<xml_diff>
--- a/resultadosPYTHON_BUBBLE.xlsx
+++ b/resultadosPYTHON_BUBBLE.xlsx
@@ -457,7 +457,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1.939058303833008</v>
+        <v>1.992702484130859</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>0</v>
@@ -468,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.881195068359375</v>
+        <v>1.101255416870117</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
@@ -479,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1.99437141418457</v>
+        <v>0.7884502410888672</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>0</v>
@@ -490,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.9980201721191406</v>
+        <v>0.995635986328125</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>0</v>
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>1.992940902709961</v>
+        <v>1.070261001586914</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>0</v>
@@ -512,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.80108642578125</v>
+        <v>0.995635986328125</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>0</v>
@@ -523,7 +523,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.9973049163818359</v>
+        <v>1.995563507080078</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>0</v>
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>2.035379409790039</v>
+        <v>0.7252693176269531</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>0</v>
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.9968280792236328</v>
+        <v>1.995325088500977</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0</v>
@@ -556,7 +556,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>1.99437141418457</v>
+        <v>1.995563507080078</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>0</v>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>1.463055610656738</v>
+        <v>1.365566253662109</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>0</v>
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.468539237976074</v>
+        <v>1.085758209228516</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>

</xml_diff>